<commit_message>
Refactor convertToExcel.py to update column headings and remove unnecessary code
</commit_message>
<xml_diff>
--- a/product_list.xlsx
+++ b/product_list.xlsx
@@ -68,15 +68,6 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="00e9ee9e"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -438,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,44 +450,20 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>ID do Produto</t>
+          <t>CR do Produto</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Categoria do Produto</t>
+          <t>Nome do Produto</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Marca do Produto</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Nome do Produto</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
           <t>Quantidade em Estoque</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Preço de Compra</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Preço de Venda</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Lucro</t>
-        </is>
-      </c>
+      <c r="D1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
@@ -504,31 +471,11 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>Aydınlatma</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>Cata</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
           <t>Masa Lambası Şarjlı</t>
         </is>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="C2" s="2" t="n">
         <v>10</v>
-      </c>
-      <c r="F2" s="2" t="n">
-        <v>50</v>
-      </c>
-      <c r="G2" s="2" t="n">
-        <v>75</v>
-      </c>
-      <c r="H2" s="2">
-        <f>G2-F2</f>
-        <v/>
       </c>
     </row>
     <row r="3">
@@ -537,31 +484,11 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>Elektrik</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>Cata</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
           <t>Su Dedektörü</t>
         </is>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="C3" s="2" t="n">
         <v>20</v>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>35</v>
-      </c>
-      <c r="G3" s="2" t="n">
-        <v>40</v>
-      </c>
-      <c r="H3" s="2">
-        <f>G3-F3</f>
-        <v/>
       </c>
     </row>
     <row r="4">
@@ -570,31 +497,11 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>Avize</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>Merivan</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="inlineStr">
-        <is>
           <t>5 Katlı Altın/Altın Lüks Avize</t>
         </is>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="C4" s="2" t="n">
         <v>1</v>
-      </c>
-      <c r="F4" s="2" t="n">
-        <v>2250</v>
-      </c>
-      <c r="G4" s="2" t="n">
-        <v>2500</v>
-      </c>
-      <c r="H4" s="2">
-        <f>G4-F4</f>
-        <v/>
       </c>
     </row>
     <row r="5">
@@ -603,31 +510,11 @@
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>Avize</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>kayseri</t>
-        </is>
-      </c>
-      <c r="D5" s="2" t="inlineStr">
-        <is>
           <t>5 Katlı Altın/Altın Lüks Avize</t>
         </is>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="C5" s="2" t="n">
         <v>2</v>
-      </c>
-      <c r="F5" s="2" t="n">
-        <v>2300</v>
-      </c>
-      <c r="G5" s="2" t="n">
-        <v>2500</v>
-      </c>
-      <c r="H5" s="2">
-        <f>G5-F5</f>
-        <v/>
       </c>
     </row>
     <row r="6">
@@ -636,31 +523,11 @@
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>Camisa</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>Poli UV</t>
-        </is>
-      </c>
-      <c r="D6" s="2" t="inlineStr">
-        <is>
           <t>5 Katlı Altın/Altın Lüks Avize</t>
         </is>
       </c>
-      <c r="E6" s="2" t="n">
+      <c r="C6" s="2" t="n">
         <v>1</v>
-      </c>
-      <c r="F6" s="2" t="n">
-        <v>2300</v>
-      </c>
-      <c r="G6" s="2" t="n">
-        <v>250</v>
-      </c>
-      <c r="H6" s="2">
-        <f>G6-F6</f>
-        <v/>
       </c>
     </row>
     <row r="7">
@@ -669,31 +536,11 @@
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>Roupa</t>
-        </is>
-      </c>
-      <c r="C7" s="2" t="inlineStr">
-        <is>
-          <t>Lacoste</t>
-        </is>
-      </c>
-      <c r="D7" s="2" t="inlineStr">
-        <is>
           <t>Camisa Polo UV</t>
         </is>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="C7" s="2" t="n">
         <v>1000</v>
-      </c>
-      <c r="F7" s="2" t="n">
-        <v>90</v>
-      </c>
-      <c r="G7" s="2" t="n">
-        <v>149</v>
-      </c>
-      <c r="H7" s="2">
-        <f>G7-F7</f>
-        <v/>
       </c>
     </row>
     <row r="8">
@@ -702,39 +549,14 @@
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>Roupas</t>
-        </is>
-      </c>
-      <c r="C8" s="2" t="inlineStr">
-        <is>
-          <t>Camisa</t>
-        </is>
-      </c>
-      <c r="D8" s="2" t="inlineStr">
-        <is>
           <t>Camisa Polo UV</t>
         </is>
       </c>
-      <c r="E8" s="2" t="n">
+      <c r="C8" s="2" t="n">
         <v>500</v>
       </c>
-      <c r="F8" s="2" t="n">
-        <v>39</v>
-      </c>
-      <c r="G8" s="2" t="n">
-        <v>79</v>
-      </c>
-      <c r="H8" s="2">
-        <f>G8-F8</f>
-        <v/>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:H8">
-    <cfRule type="expression" priority="1" dxfId="0">
-      <formula>$H1&lt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor database.py to fetch product by name and update UI to display selected item
</commit_message>
<xml_diff>
--- a/product_list.xlsx
+++ b/product_list.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,93 +467,28 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>Masa Lambası Şarjlı</t>
+          <t>xuxsss</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>10</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>Su Dedektörü</t>
+          <t>zinhos</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>5 Katlı Altın/Altın Lüks Avize</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>5 Katlı Altın/Altın Lüks Avize</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>5 Katlı Altın/Altın Lüks Avize</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="inlineStr">
-        <is>
-          <t>Camisa Polo UV</t>
-        </is>
-      </c>
-      <c r="C7" s="2" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="inlineStr">
-        <is>
-          <t>Camisa Polo UV</t>
-        </is>
-      </c>
-      <c r="C8" s="2" t="n">
-        <v>500</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>